<commit_message>
New gender budget work
</commit_message>
<xml_diff>
--- a/data/natl_budgets_value.xlsx
+++ b/data/natl_budgets_value.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="natl_budgets_value" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="percent_table" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="value_table" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="percentages" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="values" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="20">
   <si>
     <t xml:space="preserve">Principal gender equality</t>
   </si>
@@ -79,12 +79,6 @@
   </si>
   <si>
     <t xml:space="preserve">Uganda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt; 0.1%</t>
   </si>
   <si>
     <t xml:space="preserve">Total Result</t>
@@ -96,9 +90,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
-    <numFmt numFmtId="167" formatCode="0.00%"/>
+    <numFmt numFmtId="165" formatCode="0.00%"/>
+    <numFmt numFmtId="166" formatCode="@"/>
+    <numFmt numFmtId="167" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="168" formatCode="0.0%"/>
     <numFmt numFmtId="169" formatCode="0.000%"/>
     <numFmt numFmtId="170" formatCode="[$$-409]#,##0;[RED]\-[$$-409]#,##0"/>
@@ -329,12 +323,20 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -342,23 +344,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -394,7 +392,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -404,42 +402,6 @@
     </xf>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="11" xfId="21" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="6" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="9" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="22" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="23" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="24" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -539,8 +501,8 @@
   </sheetPr>
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -548,13 +510,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="8.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="6.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="16.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="20.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.08"/>
   </cols>
   <sheetData>
@@ -571,22 +531,22 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="0" t="s">
@@ -594,36 +554,36 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="0" t="n">
         <v>113038382103</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="4" t="n">
         <v>0.009</v>
       </c>
-      <c r="F2" s="3" t="n">
+      <c r="F2" s="5" t="n">
         <f aca="false">D2*E2</f>
         <v>1017345438.927</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>1651599978567</v>
       </c>
-      <c r="H2" s="3" t="n">
+      <c r="H2" s="5" t="n">
         <f aca="false">E2*G2</f>
         <v>14864399807.103</v>
       </c>
       <c r="I2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="4" t="n">
+      <c r="J2" s="1" t="n">
         <v>0.0684417435032162</v>
       </c>
       <c r="K2" s="0" t="s">
@@ -631,36 +591,36 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>113842647</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="4" t="n">
         <v>0.009</v>
       </c>
-      <c r="F3" s="3" t="n">
+      <c r="F3" s="5" t="n">
         <f aca="false">D3*E3</f>
         <v>1024583.823</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>1651599978567</v>
       </c>
-      <c r="H3" s="3" t="n">
+      <c r="H3" s="5" t="n">
         <f aca="false">E3*G3</f>
         <v>14864399807.103</v>
       </c>
       <c r="I3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="4" t="n">
+      <c r="J3" s="1" t="n">
         <v>6.89287045757744E-005</v>
       </c>
       <c r="K3" s="0" t="s">
@@ -668,36 +628,36 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="0" t="n">
         <v>18043675</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="4" t="n">
         <v>0.009</v>
       </c>
-      <c r="F4" s="3" t="n">
+      <c r="F4" s="5" t="n">
         <f aca="false">D4*E4</f>
         <v>162393.075</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>1651599978567</v>
       </c>
-      <c r="H4" s="3" t="n">
+      <c r="H4" s="5" t="n">
         <f aca="false">E4*G4</f>
         <v>14864399807.103</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="4" t="n">
+      <c r="J4" s="1" t="n">
         <v>1.09249668407331E-005</v>
       </c>
       <c r="K4" s="0" t="s">
@@ -705,110 +665,110 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>821293557505</v>
-      </c>
-      <c r="E5" s="2" t="n">
+        <v>433196090894</v>
+      </c>
+      <c r="E5" s="4" t="n">
         <v>0.0078</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="F5" s="5" t="n">
         <f aca="false">D5*E5</f>
-        <v>6406089748.539</v>
+        <v>3378929508.9732</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>19098354851073</v>
-      </c>
-      <c r="H5" s="3" t="n">
+        <v>9383760187375</v>
+      </c>
+      <c r="H5" s="5" t="n">
         <f aca="false">E5*G5</f>
-        <v>148967167838.369</v>
+        <v>73193329461.525</v>
       </c>
       <c r="I5" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="4" t="n">
-        <v>0.0430033667250066</v>
+      <c r="J5" s="1" t="n">
+        <v>0.046164446047633</v>
       </c>
       <c r="K5" s="0" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>19511778910</v>
-      </c>
-      <c r="E6" s="2" t="n">
+        <v>9755889455</v>
+      </c>
+      <c r="E6" s="4" t="n">
         <v>0.0078</v>
       </c>
-      <c r="F6" s="3" t="n">
+      <c r="F6" s="5" t="n">
         <f aca="false">D6*E6</f>
-        <v>152191875.498</v>
+        <v>76095937.749</v>
       </c>
       <c r="G6" s="0" t="n">
-        <v>19098354851073</v>
-      </c>
-      <c r="H6" s="3" t="n">
+        <v>9383760187375</v>
+      </c>
+      <c r="H6" s="5" t="n">
         <f aca="false">E6*G6</f>
-        <v>148967167838.369</v>
+        <v>73193329461.525</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="4" t="n">
-        <v>0.001021647103227</v>
+      <c r="J6" s="1" t="n">
+        <v>0.00103965673250321</v>
       </c>
       <c r="K6" s="0" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="0" t="n">
         <v>998090776960.375</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="4" t="n">
         <v>0.00027</v>
       </c>
-      <c r="F7" s="3" t="n">
+      <c r="F7" s="5" t="n">
         <f aca="false">D7*E7</f>
         <v>269484509.779301</v>
       </c>
       <c r="G7" s="0" t="n">
         <v>131056488747645</v>
       </c>
-      <c r="H7" s="3" t="n">
+      <c r="H7" s="5" t="n">
         <f aca="false">E7*G7</f>
         <v>35385251961.8641</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="4" t="n">
+      <c r="J7" s="1" t="n">
         <v>0.00761572957201869</v>
       </c>
       <c r="K7" s="0" t="s">
@@ -816,36 +776,36 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="A8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="0" t="n">
         <v>23726000</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="4" t="n">
         <v>0.00027</v>
       </c>
-      <c r="F8" s="3" t="n">
+      <c r="F8" s="5" t="n">
         <f aca="false">D8*E8</f>
         <v>6406.02</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>131056488747645</v>
       </c>
-      <c r="H8" s="3" t="n">
+      <c r="H8" s="5" t="n">
         <f aca="false">E8*G8</f>
         <v>35385251961.8641</v>
       </c>
       <c r="I8" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="4" t="n">
+      <c r="J8" s="1" t="n">
         <v>1.81036438765618E-007</v>
       </c>
       <c r="K8" s="0" t="s">
@@ -853,36 +813,36 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="0" t="n">
         <v>40000000</v>
       </c>
-      <c r="E9" s="2" t="n">
+      <c r="E9" s="4" t="n">
         <v>0.00027</v>
       </c>
-      <c r="F9" s="3" t="n">
+      <c r="F9" s="5" t="n">
         <f aca="false">D9*E9</f>
         <v>10800</v>
       </c>
       <c r="G9" s="0" t="n">
         <v>131056488747645</v>
       </c>
-      <c r="H9" s="3" t="n">
+      <c r="H9" s="5" t="n">
         <f aca="false">E9*G9</f>
         <v>35385251961.8641</v>
       </c>
       <c r="I9" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="J9" s="4" t="n">
+      <c r="J9" s="1" t="n">
         <v>3.05211900473099E-007</v>
       </c>
       <c r="K9" s="0" t="s">
@@ -905,128 +865,68 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.11"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="9" t="n">
+      <c r="B2" s="10" t="n">
         <v>0.0684417435032162</v>
       </c>
-      <c r="C2" s="10" t="n">
+      <c r="C2" s="11" t="n">
         <v>6.89287045757744E-005</v>
       </c>
-      <c r="D2" s="11" t="n">
+      <c r="D2" s="12" t="n">
         <v>1.09249668407331E-005</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="13" t="n">
-        <v>0.0430033667250066</v>
-      </c>
-      <c r="C3" s="14" t="n">
+      <c r="B3" s="14" t="n">
+        <v>0.046164446047633</v>
+      </c>
+      <c r="C3" s="15" t="n">
         <v>0</v>
       </c>
-      <c r="D3" s="15" t="n">
-        <v>0.001021647103227</v>
+      <c r="D3" s="16" t="n">
+        <v>0.00103965673250321</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="16" t="n">
+      <c r="B4" s="17" t="n">
         <v>0.00761572957201869</v>
       </c>
-      <c r="C4" s="17" t="n">
+      <c r="C4" s="18" t="n">
         <v>1.81036438765618E-007</v>
       </c>
-      <c r="D4" s="18" t="n">
+      <c r="D4" s="19" t="n">
         <v>3.05211900473099E-007</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="19" t="n">
-        <v>0.0684417435032162</v>
-      </c>
-      <c r="C8" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="21" t="n">
-        <v>0.0430033667250066</v>
-      </c>
-      <c r="C9" s="22" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" s="23" t="n">
-        <v>0.001021647103227</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="24" t="n">
-        <v>0.00761572957201869</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1047,102 +947,97 @@
   </sheetPr>
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="137" zoomScaleNormal="137" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.09"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="28" t="s">
-        <v>21</v>
+      <c r="E1" s="20" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="29" t="n">
+      <c r="B2" s="21" t="n">
         <v>1017345438.927</v>
       </c>
-      <c r="C2" s="30" t="n">
+      <c r="C2" s="22" t="n">
         <v>1024583.823</v>
       </c>
-      <c r="D2" s="31" t="n">
+      <c r="D2" s="23" t="n">
         <v>162393.075</v>
       </c>
-      <c r="E2" s="32" t="n">
+      <c r="E2" s="24" t="n">
         <v>1018532415.825</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="33" t="n">
-        <v>6406089748.539</v>
-      </c>
-      <c r="C3" s="34" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="35" t="n">
-        <v>152191875.498</v>
-      </c>
-      <c r="E3" s="36" t="n">
-        <v>6558281624.037</v>
+      <c r="B3" s="25" t="n">
+        <v>3378929508.9732</v>
+      </c>
+      <c r="C3" s="26"/>
+      <c r="D3" s="27" t="n">
+        <v>76095937.749</v>
+      </c>
+      <c r="E3" s="28" t="n">
+        <v>3455025446.7222</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="37" t="n">
+      <c r="B4" s="29" t="n">
         <v>269484509.779301</v>
       </c>
-      <c r="C4" s="38" t="n">
+      <c r="C4" s="30" t="n">
         <v>6406.02</v>
       </c>
-      <c r="D4" s="39" t="n">
+      <c r="D4" s="31" t="n">
         <v>10800</v>
       </c>
-      <c r="E4" s="40" t="n">
+      <c r="E4" s="32" t="n">
         <v>269501715.799301</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="42" t="n">
-        <v>7692919697.2453</v>
-      </c>
-      <c r="C5" s="43" t="n">
+      <c r="A5" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="34" t="n">
+        <v>4665759457.6795</v>
+      </c>
+      <c r="C5" s="35" t="n">
         <v>1030989.843</v>
       </c>
-      <c r="D5" s="44" t="n">
-        <v>152365068.573</v>
-      </c>
-      <c r="E5" s="45" t="n">
-        <v>7846315755.6613</v>
+      <c r="D5" s="36" t="n">
+        <v>76269130.824</v>
+      </c>
+      <c r="E5" s="37" t="n">
+        <v>4743059578.3465</v>
       </c>
     </row>
   </sheetData>

</xml_diff>